<commit_message>
feat: Added improved clustering and new API Key
</commit_message>
<xml_diff>
--- a/src/clustering_evaluation_metrics.xlsx
+++ b/src/clustering_evaluation_metrics.xlsx
@@ -457,16 +457,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.05737154558300972</v>
+        <v>0.04780798405408859</v>
       </c>
       <c r="B2" t="n">
-        <v>3.655686739170967</v>
+        <v>2.907422416370558</v>
       </c>
       <c r="C2" t="n">
-        <v>7.217987060546875</v>
+        <v>3.823013305664062</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BREAKING CHANGE: Latest stable version working
</commit_message>
<xml_diff>
--- a/src/clustering_evaluation_metrics.xlsx
+++ b/src/clustering_evaluation_metrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,16 +457,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.04780798405408859</v>
+        <v>0.07275096327066422</v>
       </c>
       <c r="B2" t="n">
-        <v>2.907422416370558</v>
+        <v>1.422220479928952</v>
       </c>
       <c r="C2" t="n">
-        <v>3.823013305664062</v>
+        <v>1.399654150009155</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>